<commit_message>
ya lee el excel
</commit_message>
<xml_diff>
--- a/src/public/datos.xlsx
+++ b/src/public/datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udistritaleduco-my.sharepoint.com/personal/alfgomezg_udistrital_edu_co/Documents/UNIVERSIDAD/pie 3d/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresguevara/projects/three-render/src/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F2059115-A498-4D75-9613-FBF6014DCBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58E0445B-5595-4243-95E3-9A6EC431821A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925629DD-9CC6-8440-A2AA-A17A50ABF20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11320" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
+    <workbookView xWindow="0" yWindow="9940" windowWidth="16800" windowHeight="9420" activeTab="1" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -373,9 +373,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -413,7 +413,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -519,7 +519,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -661,7 +661,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C24DED-D376-4541-996E-D47EEC06DCB7}">
   <dimension ref="A1:GQ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -12678,8 +12678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4D9A6D-2C37-4E68-91C6-C676EA5B6908}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ya lee el excel y asigna los colores con el excel
</commit_message>
<xml_diff>
--- a/src/public/datos.xlsx
+++ b/src/public/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresguevara/projects/three-render/src/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925629DD-9CC6-8440-A2AA-A17A50ABF20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DA163B-9450-FF48-A095-F7EAE1B607C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9940" windowWidth="16800" windowHeight="9420" activeTab="1" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
   </bookViews>
@@ -28,9 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -12676,10 +12679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4D9A6D-2C37-4E68-91C6-C676EA5B6908}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12688,14 +12691,14 @@
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
     </row>
-    <row r="2" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -12706,7 +12709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
@@ -12716,52 +12719,58 @@
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>48.299469964664311</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>32.791519434628974</v>
+        <f>32.791519434629+$F$3</f>
+        <v>42.791519434629002</v>
       </c>
       <c r="C5">
         <v>41.687279151943464</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>27.464664310954063</v>
+        <f>27.4646643109541+$F$3</f>
+        <v>37.464664310954099</v>
       </c>
       <c r="C6">
         <v>56.731448763250881</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>30.313604240282686</v>
+        <f>30.3136042402827+$F$3</f>
+        <v>40.3136042402827</v>
       </c>
       <c r="C7">
         <v>34.580388692579511</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -12772,7 +12781,7 @@
         <v>1.1395759717314489</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -12783,7 +12792,7 @@
         <v>76.576855123674903</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -12794,7 +12803,7 @@
         <v>102.08922261484098</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -12805,7 +12814,7 @@
         <v>77.031802120141336</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -12816,7 +12825,7 @@
         <v>73.741166077738512</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -12827,7 +12836,7 @@
         <v>45.017667844522968</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -12838,7 +12847,7 @@
         <v>31.704946996466433</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -12849,7 +12858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
v0.1.0 Tiene el pie izquierdo con el modelo 3D que tiene los 99 sensores correctos
</commit_message>
<xml_diff>
--- a/src/public/datos.xlsx
+++ b/src/public/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresguevara/projects/three-render/src/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B45F9C5-396C-0C44-BE27-DB2A7480E0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8DA8D-5A0A-DA40-B7B0-477B13D987A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9940" windowWidth="16800" windowHeight="9420" activeTab="1" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
   </bookViews>
@@ -12681,8 +12681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4D9A6D-2C37-4E68-91C6-C676EA5B6908}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12728,7 +12728,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>48.299469964664311</v>

</xml_diff>

<commit_message>
v0.1.1 los dos pies se muestran
</commit_message>
<xml_diff>
--- a/src/public/datos.xlsx
+++ b/src/public/datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresguevara/projects/three-render/src/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D8DA8D-5A0A-DA40-B7B0-477B13D987A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA940B88-8C8E-EC47-B0FC-8415FB960EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9940" windowWidth="16800" windowHeight="9420" activeTab="1" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="6" xr2:uid="{5D01DFB4-AEEC-4238-8027-960F78203D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="s4" sheetId="4" r:id="rId4"/>
     <sheet name="s5" sheetId="5" r:id="rId5"/>
     <sheet name="s6" sheetId="6" r:id="rId6"/>
+    <sheet name="s7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>LADO NO AMPUTADO</t>
   </si>
@@ -134,6 +135,9 @@
   </si>
   <si>
     <t>SUJETO S1</t>
+  </si>
+  <si>
+    <t>Prueba de colores</t>
   </si>
 </sst>
 </file>
@@ -376,9 +380,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -416,7 +420,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -522,7 +526,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -664,7 +668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -12681,8 +12685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F4D9A6D-2C37-4E68-91C6-C676EA5B6908}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13830,8 +13834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46388000-AFC0-4804-94FF-79DCCDE9FB10}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A72" zoomScale="134" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14897,7 +14901,7 @@
         <v>94</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -14908,7 +14912,7 @@
         <v>95</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C98">
         <v>17.314285714285713</v>
@@ -14919,10 +14923,10 @@
         <v>96</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -14930,7 +14934,7 @@
         <v>97</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -14941,7 +14945,7 @@
         <v>98</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -14952,7 +14956,7 @@
         <v>99</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -14970,7 +14974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C39B29-7A6E-4F8D-8D26-4E55AB1FA618}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -16112,7 +16116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414EBCB9-0A4F-4B8C-B6BB-0EE2043945DB}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A102" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
@@ -17254,7 +17258,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18387,4 +18391,1140 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDF4C03-B3BA-1140-B755-77AE3DD0219E}">
+  <dimension ref="A1:C102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="C39">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="C40">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="C41">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>41</v>
+      </c>
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>42</v>
+      </c>
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="C49">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="C51">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="9">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="9">
+        <v>51</v>
+      </c>
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="C54">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="9">
+        <v>52</v>
+      </c>
+      <c r="B55">
+        <v>52</v>
+      </c>
+      <c r="C55">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="9">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>53</v>
+      </c>
+      <c r="C56">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="9">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="9">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="9">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="C59">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="9">
+        <v>57</v>
+      </c>
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="C60">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="9">
+        <v>58</v>
+      </c>
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="C61">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="9">
+        <v>59</v>
+      </c>
+      <c r="B62">
+        <v>59</v>
+      </c>
+      <c r="C62">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="9">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="9">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <v>61</v>
+      </c>
+      <c r="C64">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="9">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>62</v>
+      </c>
+      <c r="C65">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="9">
+        <v>63</v>
+      </c>
+      <c r="B66">
+        <v>63</v>
+      </c>
+      <c r="C66">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="9">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>64</v>
+      </c>
+      <c r="C67">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="9">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <v>65</v>
+      </c>
+      <c r="C68">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="9">
+        <v>66</v>
+      </c>
+      <c r="B69">
+        <v>66</v>
+      </c>
+      <c r="C69">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>67</v>
+      </c>
+      <c r="C70">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="9">
+        <v>68</v>
+      </c>
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="C71">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="9">
+        <v>69</v>
+      </c>
+      <c r="B72">
+        <v>69</v>
+      </c>
+      <c r="C72">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="9">
+        <v>70</v>
+      </c>
+      <c r="B73">
+        <v>70</v>
+      </c>
+      <c r="C73">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="9">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>71</v>
+      </c>
+      <c r="C74">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="9">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <v>72</v>
+      </c>
+      <c r="C75">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="9">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <v>73</v>
+      </c>
+      <c r="C76">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="9">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>74</v>
+      </c>
+      <c r="C77">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="9">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <v>75</v>
+      </c>
+      <c r="C78">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="9">
+        <v>76</v>
+      </c>
+      <c r="B79">
+        <v>76</v>
+      </c>
+      <c r="C79">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="9">
+        <v>77</v>
+      </c>
+      <c r="B80">
+        <v>77</v>
+      </c>
+      <c r="C80">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="9">
+        <v>78</v>
+      </c>
+      <c r="B81">
+        <v>78</v>
+      </c>
+      <c r="C81">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="9">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>79</v>
+      </c>
+      <c r="C82">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="9">
+        <v>80</v>
+      </c>
+      <c r="B83">
+        <v>80</v>
+      </c>
+      <c r="C83">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="9">
+        <v>81</v>
+      </c>
+      <c r="B84">
+        <v>81</v>
+      </c>
+      <c r="C84">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="9">
+        <v>82</v>
+      </c>
+      <c r="B85">
+        <v>82</v>
+      </c>
+      <c r="C85">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="9">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <v>83</v>
+      </c>
+      <c r="C86">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="9">
+        <v>84</v>
+      </c>
+      <c r="B87">
+        <v>84</v>
+      </c>
+      <c r="C87">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="9">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>85</v>
+      </c>
+      <c r="C88">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="9">
+        <v>86</v>
+      </c>
+      <c r="B89">
+        <v>86</v>
+      </c>
+      <c r="C89">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="9">
+        <v>87</v>
+      </c>
+      <c r="B90">
+        <v>87</v>
+      </c>
+      <c r="C90">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="9">
+        <v>88</v>
+      </c>
+      <c r="B91">
+        <v>88</v>
+      </c>
+      <c r="C91">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="9">
+        <v>89</v>
+      </c>
+      <c r="B92">
+        <v>89</v>
+      </c>
+      <c r="C92">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="9">
+        <v>90</v>
+      </c>
+      <c r="B93">
+        <v>90</v>
+      </c>
+      <c r="C93">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="9">
+        <v>91</v>
+      </c>
+      <c r="B94">
+        <v>91</v>
+      </c>
+      <c r="C94">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="9">
+        <v>92</v>
+      </c>
+      <c r="B95">
+        <v>92</v>
+      </c>
+      <c r="C95">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="9">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <v>93</v>
+      </c>
+      <c r="C96">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="9">
+        <v>94</v>
+      </c>
+      <c r="B97">
+        <v>94</v>
+      </c>
+      <c r="C97">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="9">
+        <v>95</v>
+      </c>
+      <c r="B98">
+        <v>95</v>
+      </c>
+      <c r="C98">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="9">
+        <v>96</v>
+      </c>
+      <c r="B99">
+        <v>96</v>
+      </c>
+      <c r="C99">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="9">
+        <v>97</v>
+      </c>
+      <c r="B100">
+        <v>97</v>
+      </c>
+      <c r="C100">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="9">
+        <v>98</v>
+      </c>
+      <c r="B101">
+        <v>98</v>
+      </c>
+      <c r="C101">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="11">
+        <v>99</v>
+      </c>
+      <c r="B102">
+        <v>99</v>
+      </c>
+      <c r="C102">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>